<commit_message>
Matriz de trazabilidad 1
</commit_message>
<xml_diff>
--- a/02.Implementación de proyecto/Primer Sprint/SGySHT_ReporteSprint1_v1.xlsx
+++ b/02.Implementación de proyecto/Primer Sprint/SGySHT_ReporteSprint1_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SoyAleZamora\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SoyAleZamora\Desktop\Proyecto_SGySHT\Proyecto_SGySHT\02.Implementación de proyecto\Primer Sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1541,6 +1541,35 @@
   <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Fecha</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" baseline="0"/>
+              <a:t>  de finalización estimal y actual</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3854,9 +3883,9 @@
   </sheetPr>
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>